<commit_message>
"Modified automation for Api data setup"
</commit_message>
<xml_diff>
--- a/src/test/resources/data/JobData.xlsx
+++ b/src/test/resources/data/JobData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>title</t>
   </si>
@@ -35,24 +35,12 @@
     <t>Architect</t>
   </si>
   <si>
-    <t>Technical Architect - Birmingham - Circa £65K C#, .NET. Our growing client based near Manchester is currently looking for a skilled Technical Architect.The role will be to provide leadership in technologies, system design</t>
-  </si>
-  <si>
     <t>location</t>
   </si>
   <si>
     <t>Birmingham</t>
   </si>
   <si>
-    <t>salMin</t>
-  </si>
-  <si>
-    <t>salMax</t>
-  </si>
-  <si>
-    <t>noOfVacancies</t>
-  </si>
-  <si>
     <t>closingDate</t>
   </si>
   <si>
@@ -110,25 +98,73 @@
     <t>BusinessAnalyst</t>
   </si>
   <si>
-    <t>BusinessAnalyst - Cardiff - Circa £65K C#, .NET. Our growing client based near Manchester is currently looking for a skilled Technical Architect.The role will be to provide leadership in technologies, system design</t>
-  </si>
-  <si>
-    <t>50000</t>
-  </si>
-  <si>
-    <t>20-10-18</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
     <t>role is role</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Swindon</t>
+  </si>
+  <si>
+    <t>department/id</t>
+  </si>
+  <si>
+    <t>department/name</t>
+  </si>
+  <si>
+    <t>﻿HM revenue and customs</t>
+  </si>
+  <si>
+    <t>﻿Department for Works and pensions</t>
+  </si>
+  <si>
+    <t>﻿Department of transport</t>
+  </si>
+  <si>
+    <t>Auto-Technical Architect - Birmingham - Circa £65K C#, .NET. Our growing client based near Manchester is currently looking for a skilled Technical Architect.The role will be to provide leadership in technologies, system design</t>
+  </si>
+  <si>
+    <t>Auto-BusinessAnalyst - Cardiff - Circa £65K C#, .NET. Our growing client based near Manchester is currently looking for a skilled Technical Architect.The role will be to provide leadership in technologies, system design</t>
+  </si>
+  <si>
+    <t>2018-02-21T14:30:43.014+0000</t>
+  </si>
+  <si>
+    <t>2018-01-21T14:30:43.014+0000</t>
+  </si>
+  <si>
+    <t>publicOpeningDate</t>
+  </si>
+  <si>
+    <t>governmentOpeningDate</t>
+  </si>
+  <si>
+    <t>internalOpeningDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>salaryMin</t>
+  </si>
+  <si>
+    <t>salaryMax</t>
+  </si>
+  <si>
+    <t>numberVacancies</t>
+  </si>
+  <si>
+    <t>Department of animal sciences</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -186,10 +222,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -205,6 +243,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -473,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,219 +525,343 @@
     <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="2" max="2" width="53.1640625" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="14" max="14" width="14.5" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" customWidth="1"/>
+    <col min="7" max="10" width="27.83203125" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="21" max="21" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" t="s">
-        <v>22</v>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>30000</v>
+      </c>
+      <c r="E2" s="3">
+        <v>50000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3">
+        <v>50000</v>
+      </c>
+      <c r="E3" s="3">
+        <v>50000</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="3">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
-        <v>30000</v>
-      </c>
-      <c r="E2" s="1">
-        <v>50000</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="1">
-        <v>50000</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3">
         <v>30000</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>50000</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
+      <c r="F4" s="4">
+        <v>45</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3">
+        <v>30000</v>
+      </c>
+      <c r="E5" s="3">
+        <v>50000</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="P5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>23</v>
+      <c r="T5" s="3">
+        <v>11</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="G2:G3" twoDigitTextYear="1"/>
-    <ignoredError sqref="D3" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>